<commit_message>
first draft of TripBuilder. Known trip break bug
</commit_message>
<xml_diff>
--- a/TEST_CASES.xlsx
+++ b/TEST_CASES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24822"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kniggee\Downloads\tolldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE2AACD-6B17-499B-AC37-7DE2A6B9FC1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0FE80E1F-C36B-4F8D-866A-DEAD547E5BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="travel_time" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -247,10 +248,10 @@
     <t>t8 + delta * 2</t>
   </si>
   <si>
-    <t>t8 + timeout + delta</t>
-  </si>
-  <si>
-    <t>t8 + timeout + delta*2</t>
+    <t>t8 + timeout + delta*3</t>
+  </si>
+  <si>
+    <t>t8 + timeout + delta*4</t>
   </si>
   <si>
     <t>NEC2057</t>
@@ -283,12 +284,15 @@
     <t>t10 + timeout + delta * 2</t>
   </si>
   <si>
+    <t>ATG8613</t>
+  </si>
+  <si>
+    <t>plate misread, tag intermittent</t>
+  </si>
+  <si>
     <t>t11</t>
   </si>
   <si>
-    <t>ATG8613</t>
-  </si>
-  <si>
     <t>4TG8613</t>
   </si>
   <si>
@@ -296,16 +300,13 @@
   </si>
   <si>
     <t>ATGB6I3</t>
-  </si>
-  <si>
-    <t>plate misread, tag intermittent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -693,12 +694,12 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="5" max="5" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:12">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -712,7 +713,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:12">
       <c r="C5">
         <v>1</v>
       </c>
@@ -732,7 +733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:12">
       <c r="C6">
         <v>1</v>
       </c>
@@ -753,7 +754,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:12">
       <c r="C7">
         <v>1</v>
       </c>
@@ -775,7 +776,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:12">
       <c r="C8">
         <v>1</v>
       </c>
@@ -797,7 +798,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:12">
       <c r="C9">
         <v>1</v>
       </c>
@@ -819,7 +820,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:12">
       <c r="C10">
         <v>1</v>
       </c>
@@ -841,7 +842,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:12">
       <c r="C11">
         <v>1</v>
       </c>
@@ -863,7 +864,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:12">
       <c r="C12">
         <v>2</v>
       </c>
@@ -878,7 +879,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:12">
       <c r="C13">
         <v>2</v>
       </c>
@@ -893,7 +894,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:12">
       <c r="C14">
         <v>3</v>
       </c>
@@ -908,7 +909,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:12">
       <c r="C15">
         <v>3</v>
       </c>
@@ -923,7 +924,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:12">
       <c r="C16">
         <v>4</v>
       </c>
@@ -938,7 +939,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:12">
       <c r="C17">
         <v>4</v>
       </c>
@@ -960,7 +961,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:12">
       <c r="K18">
         <v>1000</v>
       </c>
@@ -968,7 +969,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:12">
       <c r="K19">
         <f>K17*K18</f>
         <v>10.48951048951049</v>
@@ -986,11 +987,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA22AA11-1B2C-4E68-99B2-4263A24ADFF0}">
   <dimension ref="C2:Q54"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48:I54"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="22" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" customWidth="1"/>
@@ -1004,7 +1005,7 @@
     <col min="17" max="17" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:17">
       <c r="C2" s="1" t="s">
         <v>22</v>
       </c>
@@ -1042,7 +1043,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:17">
       <c r="C3" s="1">
         <v>1</v>
       </c>
@@ -1080,7 +1081,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:17">
       <c r="C4" s="1">
         <v>2</v>
       </c>
@@ -1120,7 +1121,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:17">
       <c r="C5" s="1">
         <v>3</v>
       </c>
@@ -1160,7 +1161,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:17">
       <c r="C6" s="1">
         <v>4</v>
       </c>
@@ -1200,7 +1201,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:17">
       <c r="C7" s="1">
         <v>5</v>
       </c>
@@ -1240,7 +1241,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:17">
       <c r="C8" s="1">
         <v>6</v>
       </c>
@@ -1277,7 +1278,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:17">
       <c r="C9" s="1">
         <v>7</v>
       </c>
@@ -1314,7 +1315,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:17">
       <c r="C10" s="1">
         <v>8</v>
       </c>
@@ -1352,7 +1353,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:17">
       <c r="C11" s="1">
         <v>9</v>
       </c>
@@ -1392,7 +1393,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:17">
       <c r="C12" s="1">
         <v>10</v>
       </c>
@@ -1432,7 +1433,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:17">
       <c r="C13" s="1">
         <v>11</v>
       </c>
@@ -1472,7 +1473,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:17">
       <c r="C14" s="1">
         <v>12</v>
       </c>
@@ -1512,7 +1513,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:17">
       <c r="C15" s="1">
         <v>13</v>
       </c>
@@ -1544,7 +1545,7 @@
       </c>
       <c r="N15">
         <f ca="1">RANDBETWEEN(1111,99999)</f>
-        <v>88175</v>
+        <v>73051</v>
       </c>
       <c r="P15" t="s">
         <v>47</v>
@@ -1553,7 +1554,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:17">
       <c r="C16" s="1">
         <v>14</v>
       </c>
@@ -1588,7 +1589,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:17">
       <c r="C17" s="1">
         <v>15</v>
       </c>
@@ -1617,7 +1618,7 @@
       </c>
       <c r="N17" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(1111,9999)</f>
-        <v>ATW5067</v>
+        <v>SIK1533</v>
       </c>
       <c r="P17" t="s">
         <v>53</v>
@@ -1626,7 +1627,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:17">
       <c r="C18" s="1">
         <v>16</v>
       </c>
@@ -1660,7 +1661,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:17">
       <c r="C19" s="1">
         <v>17</v>
       </c>
@@ -1695,7 +1696,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:17">
       <c r="C20" s="1">
         <v>18</v>
       </c>
@@ -1732,7 +1733,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:17">
       <c r="C21" s="1">
         <v>19</v>
       </c>
@@ -1769,7 +1770,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:17">
       <c r="C22" s="1">
         <v>20</v>
       </c>
@@ -1806,7 +1807,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:17">
       <c r="C23" s="1">
         <v>21</v>
       </c>
@@ -1843,7 +1844,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:17">
       <c r="C24" s="1">
         <v>22</v>
       </c>
@@ -1874,7 +1875,7 @@
         <v>t4 + delta*6</v>
       </c>
     </row>
-    <row r="25" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:17">
       <c r="C25" s="1">
         <v>23</v>
       </c>
@@ -1905,7 +1906,7 @@
         <v>t4 + delta*7</v>
       </c>
     </row>
-    <row r="26" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:17">
       <c r="C26" s="1">
         <v>24</v>
       </c>
@@ -1936,7 +1937,7 @@
         <v>t4 + delta*8</v>
       </c>
     </row>
-    <row r="27" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:17">
       <c r="C27" s="1">
         <v>25</v>
       </c>
@@ -1965,7 +1966,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:17">
       <c r="C28" s="1">
         <v>26</v>
       </c>
@@ -1996,7 +1997,7 @@
         <v>t5 + delta*2</v>
       </c>
     </row>
-    <row r="29" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:17">
       <c r="C29" s="1">
         <v>27</v>
       </c>
@@ -2027,7 +2028,7 @@
         <v>t5 + delta*3</v>
       </c>
     </row>
-    <row r="30" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:17">
       <c r="C30" s="1">
         <v>28</v>
       </c>
@@ -2058,7 +2059,7 @@
         <v>t5 + delta*4</v>
       </c>
     </row>
-    <row r="31" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:17">
       <c r="C31" s="1">
         <v>29</v>
       </c>
@@ -2084,7 +2085,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:17">
       <c r="C32" s="1">
         <v>30</v>
       </c>
@@ -2113,7 +2114,7 @@
         <v>t6 + detal*2</v>
       </c>
     </row>
-    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:11">
       <c r="C33" s="1">
         <v>31</v>
       </c>
@@ -2141,7 +2142,7 @@
         <v>t6 + detal*3</v>
       </c>
     </row>
-    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:11">
       <c r="C34" s="1">
         <v>32</v>
       </c>
@@ -2170,7 +2171,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:11">
       <c r="C35" s="1">
         <v>33</v>
       </c>
@@ -2201,7 +2202,7 @@
         <v>t7 + delta*2</v>
       </c>
     </row>
-    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:11">
       <c r="C36" s="1">
         <v>34</v>
       </c>
@@ -2229,7 +2230,7 @@
         <v>t7 + delta*3</v>
       </c>
     </row>
-    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:11">
       <c r="C37" s="1">
         <v>35</v>
       </c>
@@ -2258,7 +2259,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:11">
       <c r="C38" s="1">
         <v>36</v>
       </c>
@@ -2288,13 +2289,13 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:11">
       <c r="C39" s="1">
         <v>37</v>
       </c>
       <c r="D39" s="2">
-        <f>D37+N13+N11</f>
-        <v>44197.354861111118</v>
+        <f>D37+N13+N11*3</f>
+        <v>44197.356250000004</v>
       </c>
       <c r="E39" t="s">
         <v>4</v>
@@ -2318,13 +2319,13 @@
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:11">
       <c r="C40" s="1">
         <v>38</v>
       </c>
       <c r="D40" s="2">
         <f>D39+N11</f>
-        <v>44197.355555555565</v>
+        <v>44197.356944444451</v>
       </c>
       <c r="E40" t="s">
         <v>6</v>
@@ -2348,7 +2349,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:11">
       <c r="C41" s="1">
         <v>39</v>
       </c>
@@ -2377,7 +2378,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:11">
       <c r="C42" s="1">
         <v>40</v>
       </c>
@@ -2407,7 +2408,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:11">
       <c r="C43" s="1">
         <v>41</v>
       </c>
@@ -2437,7 +2438,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="44" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:11">
       <c r="C44" s="1">
         <v>42</v>
       </c>
@@ -2467,7 +2468,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:11">
       <c r="C45" s="1">
         <v>43</v>
       </c>
@@ -2496,7 +2497,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="46" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:11">
       <c r="C46" s="1">
         <v>44</v>
       </c>
@@ -2526,7 +2527,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:11">
       <c r="C47" s="1">
         <v>45</v>
       </c>
@@ -2556,7 +2557,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="48" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:11">
       <c r="C48" s="1">
         <v>46</v>
       </c>
@@ -2567,7 +2568,7 @@
         <v>4</v>
       </c>
       <c r="F48" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G48">
         <v>83708</v>
@@ -2576,16 +2577,16 @@
         <v>15</v>
       </c>
       <c r="I48" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="J48">
         <v>11</v>
       </c>
       <c r="K48" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="49" spans="3:11" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="49" spans="3:11">
       <c r="C49" s="1">
         <v>47</v>
       </c>
@@ -2597,13 +2598,13 @@
         <v>6</v>
       </c>
       <c r="F49" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H49">
         <v>15</v>
       </c>
       <c r="I49" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="J49">
         <v>11</v>
@@ -2613,7 +2614,7 @@
         <v>t11 + delta</v>
       </c>
     </row>
-    <row r="50" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:11">
       <c r="C50" s="1">
         <v>48</v>
       </c>
@@ -2625,13 +2626,13 @@
         <v>8</v>
       </c>
       <c r="F50" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H50">
         <v>15</v>
       </c>
       <c r="I50" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="J50">
         <v>11</v>
@@ -2641,7 +2642,7 @@
         <v>t11 + delta * 2</v>
       </c>
     </row>
-    <row r="51" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:11">
       <c r="C51" s="1">
         <v>49</v>
       </c>
@@ -2653,13 +2654,13 @@
         <v>10</v>
       </c>
       <c r="F51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H51">
         <v>15</v>
       </c>
       <c r="I51" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="J51">
         <v>11</v>
@@ -2669,7 +2670,7 @@
         <v>t11 + delta * 3</v>
       </c>
     </row>
-    <row r="52" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:11">
       <c r="C52" s="1">
         <v>50</v>
       </c>
@@ -2681,7 +2682,7 @@
         <v>12</v>
       </c>
       <c r="F52" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G52">
         <v>83708</v>
@@ -2690,7 +2691,7 @@
         <v>15</v>
       </c>
       <c r="I52" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="J52">
         <v>11</v>
@@ -2700,7 +2701,7 @@
         <v>t11 + delta * 4</v>
       </c>
     </row>
-    <row r="53" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:11">
       <c r="C53" s="1">
         <v>51</v>
       </c>
@@ -2712,13 +2713,13 @@
         <v>14</v>
       </c>
       <c r="F53" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H53">
         <v>15</v>
       </c>
       <c r="I53" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="J53">
         <v>11</v>
@@ -2728,7 +2729,7 @@
         <v>t11 + delta * 5</v>
       </c>
     </row>
-    <row r="54" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:11">
       <c r="C54" s="1">
         <v>52</v>
       </c>
@@ -2740,7 +2741,7 @@
         <v>16</v>
       </c>
       <c r="F54" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G54">
         <v>83708</v>
@@ -2749,7 +2750,7 @@
         <v>15</v>
       </c>
       <c r="I54" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="J54">
         <v>11</v>
@@ -2768,24 +2769,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E40FFED-CB0E-47B0-9F9C-3A9A83B0082D}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I54" sqref="A54:I62"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="str">
         <f>trip_building!C2</f>
         <v>TRANSACTION_ID</v>
@@ -2823,12 +2824,12 @@
         <v>TIME_DESCRIPTION</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2">
         <f>trip_building!C3</f>
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <f>trip_building!D3</f>
         <v>44197.208333333336</v>
       </c>
@@ -2861,12 +2862,12 @@
         <v>t1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3">
         <f>trip_building!C4</f>
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <f>trip_building!D4</f>
         <v>44197.209722222222</v>
       </c>
@@ -2899,12 +2900,12 @@
         <v>t1 + delta*2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4">
         <f>trip_building!C5</f>
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <f>trip_building!D5</f>
         <v>44197.210416666669</v>
       </c>
@@ -2937,12 +2938,12 @@
         <v>t1 + delta*3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5">
         <f>trip_building!C6</f>
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <f>trip_building!D6</f>
         <v>44197.211111111115</v>
       </c>
@@ -2975,12 +2976,12 @@
         <v>t1 + delta*4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6">
         <f>trip_building!C7</f>
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <f>trip_building!D7</f>
         <v>44197.211805555555</v>
       </c>
@@ -3013,12 +3014,12 @@
         <v>t1 + delta*5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7">
         <f>trip_building!C8</f>
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <f>trip_building!D8</f>
         <v>44197.212500000001</v>
       </c>
@@ -3051,12 +3052,12 @@
         <v>t1 + delta*6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8">
         <f>trip_building!C9</f>
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <f>trip_building!D9</f>
         <v>44197.213194444448</v>
       </c>
@@ -3089,12 +3090,12 @@
         <v>t1 + delta*7</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9">
         <f>trip_building!C10</f>
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <f>trip_building!D10</f>
         <v>44197.583333333336</v>
       </c>
@@ -3127,12 +3128,12 @@
         <v>t2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10">
         <f>trip_building!C11</f>
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <f>trip_building!D11</f>
         <v>44197.584722222222</v>
       </c>
@@ -3165,12 +3166,12 @@
         <v>t2  + delta*2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11">
         <f>trip_building!C12</f>
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <f>trip_building!D12</f>
         <v>44197.585416666669</v>
       </c>
@@ -3203,12 +3204,12 @@
         <v>t2  + delta*3</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12">
         <f>trip_building!C13</f>
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <f>trip_building!D13</f>
         <v>44197.586111111115</v>
       </c>
@@ -3241,12 +3242,12 @@
         <v>t2  + delta*4</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13">
         <f>trip_building!C14</f>
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <f>trip_building!D14</f>
         <v>44197.586805555555</v>
       </c>
@@ -3279,12 +3280,12 @@
         <v>t2  + delta*5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14">
         <f>trip_building!C15</f>
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="2">
         <f>trip_building!D15</f>
         <v>44197.587500000001</v>
       </c>
@@ -3317,12 +3318,12 @@
         <v>t2  + delta*6</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15">
         <f>trip_building!C16</f>
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2">
         <f>trip_building!D16</f>
         <v>44197.416666666664</v>
       </c>
@@ -3334,10 +3335,6 @@
         <f>trip_building!F16</f>
         <v>AOG7894</v>
       </c>
-      <c r="E15">
-        <f>trip_building!G16</f>
-        <v>0</v>
-      </c>
       <c r="F15">
         <f>trip_building!H16</f>
         <v>4</v>
@@ -3355,12 +3352,12 @@
         <v>t3</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16">
         <f>trip_building!C17</f>
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
         <f>trip_building!D17</f>
         <v>44197.41805555555</v>
       </c>
@@ -3372,10 +3369,6 @@
         <f>trip_building!F17</f>
         <v>AQG7894</v>
       </c>
-      <c r="E16">
-        <f>trip_building!G17</f>
-        <v>0</v>
-      </c>
       <c r="F16">
         <f>trip_building!H17</f>
         <v>4</v>
@@ -3393,12 +3386,12 @@
         <v>t3 + delta*2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17">
         <f>trip_building!C18</f>
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <f>trip_building!D18</f>
         <v>44197.418749999997</v>
       </c>
@@ -3410,10 +3403,6 @@
         <f>trip_building!F18</f>
         <v>AOG7894</v>
       </c>
-      <c r="E17">
-        <f>trip_building!G18</f>
-        <v>0</v>
-      </c>
       <c r="F17">
         <f>trip_building!H18</f>
         <v>4</v>
@@ -3431,12 +3420,12 @@
         <v>t3 + delta*3</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18">
         <f>trip_building!C19</f>
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
         <f>trip_building!D19</f>
         <v>44197.520833333336</v>
       </c>
@@ -3469,12 +3458,12 @@
         <v>t4</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19">
         <f>trip_building!C20</f>
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="2">
         <f>trip_building!D20</f>
         <v>44197.522222222222</v>
       </c>
@@ -3507,12 +3496,12 @@
         <v>t4 + delta*2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20">
         <f>trip_building!C21</f>
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="2">
         <f>trip_building!D21</f>
         <v>44197.522916666669</v>
       </c>
@@ -3545,12 +3534,12 @@
         <v>t4 + delta*3</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21">
         <f>trip_building!C22</f>
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="2">
         <f>trip_building!D22</f>
         <v>44197.523611111115</v>
       </c>
@@ -3583,12 +3572,12 @@
         <v>t4 + delta*4</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22">
         <f>trip_building!C23</f>
         <v>21</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="2">
         <f>trip_building!D23</f>
         <v>44197.524305555555</v>
       </c>
@@ -3621,12 +3610,12 @@
         <v>t4 + delta*5</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23">
         <f>trip_building!C24</f>
         <v>22</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="2">
         <f>trip_building!D24</f>
         <v>44197.525000000001</v>
       </c>
@@ -3659,12 +3648,12 @@
         <v>t4 + delta*6</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24">
         <f>trip_building!C25</f>
         <v>23</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="2">
         <f>trip_building!D25</f>
         <v>44197.525694444448</v>
       </c>
@@ -3697,12 +3686,12 @@
         <v>t4 + delta*7</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25">
         <f>trip_building!C26</f>
         <v>24</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="2">
         <f>trip_building!D26</f>
         <v>44197.526388888895</v>
       </c>
@@ -3735,12 +3724,12 @@
         <v>t4 + delta*8</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="A26">
         <f>trip_building!C27</f>
         <v>25</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="2">
         <f>trip_building!D27</f>
         <v>44197.368055555555</v>
       </c>
@@ -3773,12 +3762,12 @@
         <v>t5</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="A27">
         <f>trip_building!C28</f>
         <v>26</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="2">
         <f>trip_building!D28</f>
         <v>44197.369444444441</v>
       </c>
@@ -3811,12 +3800,12 @@
         <v>t5 + delta*2</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28">
         <f>trip_building!C29</f>
         <v>27</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="2">
         <f>trip_building!D29</f>
         <v>44197.370138888888</v>
       </c>
@@ -3849,12 +3838,12 @@
         <v>t5 + delta*3</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29">
         <f>trip_building!C30</f>
         <v>28</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="2">
         <f>trip_building!D30</f>
         <v>44197.370833333334</v>
       </c>
@@ -3887,12 +3876,12 @@
         <v>t5 + delta*4</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="A30">
         <f>trip_building!C31</f>
         <v>29</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="2">
         <f>trip_building!D31</f>
         <v>44197.458333333336</v>
       </c>
@@ -3904,10 +3893,6 @@
         <f>trip_building!F31</f>
         <v>IAB8379</v>
       </c>
-      <c r="E30">
-        <f>trip_building!G31</f>
-        <v>0</v>
-      </c>
       <c r="F30">
         <f>trip_building!H31</f>
         <v>8</v>
@@ -3925,12 +3910,12 @@
         <v>t6</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="A31">
         <f>trip_building!C32</f>
         <v>30</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="2">
         <f>trip_building!D32</f>
         <v>44197.459722222222</v>
       </c>
@@ -3942,10 +3927,6 @@
         <f>trip_building!F32</f>
         <v>1488379</v>
       </c>
-      <c r="E31">
-        <f>trip_building!G32</f>
-        <v>0</v>
-      </c>
       <c r="F31">
         <f>trip_building!H32</f>
         <v>8</v>
@@ -3963,12 +3944,12 @@
         <v>t6 + detal*2</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9">
       <c r="A32">
         <f>trip_building!C33</f>
         <v>31</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="2">
         <f>trip_building!D33</f>
         <v>44197.460416666669</v>
       </c>
@@ -3980,10 +3961,6 @@
         <f>trip_building!F33</f>
         <v>IABB379</v>
       </c>
-      <c r="E32">
-        <f>trip_building!G33</f>
-        <v>0</v>
-      </c>
       <c r="F32">
         <f>trip_building!H33</f>
         <v>8</v>
@@ -4001,12 +3978,12 @@
         <v>t6 + detal*3</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9">
       <c r="A33">
         <f>trip_building!C34</f>
         <v>32</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="2">
         <f>trip_building!D34</f>
         <v>44197.631944444445</v>
       </c>
@@ -4039,12 +4016,12 @@
         <v>t7</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9">
       <c r="A34">
         <f>trip_building!C35</f>
         <v>33</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="2">
         <f>trip_building!D35</f>
         <v>44197.633333333331</v>
       </c>
@@ -4077,12 +4054,12 @@
         <v>t7 + delta*2</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9">
       <c r="A35">
         <f>trip_building!C36</f>
         <v>34</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="2">
         <f>trip_building!D36</f>
         <v>44197.634027777778</v>
       </c>
@@ -4094,10 +4071,6 @@
         <f>trip_building!F36</f>
         <v>4GM39A2</v>
       </c>
-      <c r="E35">
-        <f>trip_building!G36</f>
-        <v>0</v>
-      </c>
       <c r="F35">
         <f>trip_building!H36</f>
         <v>9</v>
@@ -4115,12 +4088,12 @@
         <v>t7 + delta*3</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9">
       <c r="A36">
         <f>trip_building!C37</f>
         <v>35</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="2">
         <f>trip_building!D37</f>
         <v>44197.333333333336</v>
       </c>
@@ -4153,12 +4126,12 @@
         <v>t8</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9">
       <c r="A37">
         <f>trip_building!C38</f>
         <v>36</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="2">
         <f>trip_building!D38</f>
         <v>44197.334722222222</v>
       </c>
@@ -4191,14 +4164,14 @@
         <v>t8 + delta * 2</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9">
       <c r="A38">
         <f>trip_building!C39</f>
         <v>37</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="2">
         <f>trip_building!D39</f>
-        <v>44197.354861111118</v>
+        <v>44197.356250000004</v>
       </c>
       <c r="C38" t="str">
         <f>trip_building!E39</f>
@@ -4226,17 +4199,17 @@
       </c>
       <c r="I38" t="str">
         <f>trip_building!K39</f>
-        <v>t8 + timeout + delta</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+        <v>t8 + timeout + delta*3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39">
         <f>trip_building!C40</f>
         <v>38</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="2">
         <f>trip_building!D40</f>
-        <v>44197.355555555565</v>
+        <v>44197.356944444451</v>
       </c>
       <c r="C39" t="str">
         <f>trip_building!E40</f>
@@ -4264,15 +4237,15 @@
       </c>
       <c r="I39" t="str">
         <f>trip_building!K40</f>
-        <v>t8 + timeout + delta*2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>t8 + timeout + delta*4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40">
         <f>trip_building!C41</f>
         <v>39</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="2">
         <f>trip_building!D41</f>
         <v>44197.260416666664</v>
       </c>
@@ -4305,12 +4278,12 @@
         <v>t9</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9">
       <c r="A41">
         <f>trip_building!C42</f>
         <v>40</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="2">
         <f>trip_building!D42</f>
         <v>44197.26180555555</v>
       </c>
@@ -4343,12 +4316,12 @@
         <v>t9 + delta</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9">
       <c r="A42">
         <f>trip_building!C43</f>
         <v>41</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="2">
         <f>trip_building!D43</f>
         <v>44197.262499999997</v>
       </c>
@@ -4381,12 +4354,12 @@
         <v>t9 + delta *2</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9">
       <c r="A43">
         <f>trip_building!C44</f>
         <v>42</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="2">
         <f>trip_building!D44</f>
         <v>44197.263194444444</v>
       </c>
@@ -4419,12 +4392,12 @@
         <v>t9 + delta * 3</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9">
       <c r="A44">
         <f>trip_building!C45</f>
         <v>43</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="2">
         <f>trip_building!D45</f>
         <v>44197.322916666664</v>
       </c>
@@ -4457,12 +4430,12 @@
         <v>t10</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9">
       <c r="A45">
         <f>trip_building!C46</f>
         <v>44</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="2">
         <f>trip_building!D46</f>
         <v>44197.344444444447</v>
       </c>
@@ -4495,12 +4468,12 @@
         <v>t10 + timeout + delta</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9">
       <c r="A46">
         <f>trip_building!C47</f>
         <v>45</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="2">
         <f>trip_building!D47</f>
         <v>44197.345138888893</v>
       </c>
@@ -4533,12 +4506,12 @@
         <v>t10 + timeout + delta * 2</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9">
       <c r="A47">
         <f>trip_building!C48</f>
         <v>46</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="2">
         <f>trip_building!D48</f>
         <v>44197.385416666664</v>
       </c>
@@ -4571,12 +4544,12 @@
         <v>t11</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9">
       <c r="A48">
         <f>trip_building!C49</f>
         <v>47</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="2">
         <f>trip_building!D49</f>
         <v>44197.386111111111</v>
       </c>
@@ -4588,10 +4561,6 @@
         <f>trip_building!F49</f>
         <v>4TG8613</v>
       </c>
-      <c r="E48">
-        <f>trip_building!G49</f>
-        <v>0</v>
-      </c>
       <c r="F48">
         <f>trip_building!H49</f>
         <v>15</v>
@@ -4609,12 +4578,12 @@
         <v>t11 + delta</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9">
       <c r="A49">
         <f>trip_building!C50</f>
         <v>48</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="2">
         <f>trip_building!D50</f>
         <v>44197.38680555555</v>
       </c>
@@ -4626,10 +4595,6 @@
         <f>trip_building!F50</f>
         <v>ATGB613</v>
       </c>
-      <c r="E49">
-        <f>trip_building!G50</f>
-        <v>0</v>
-      </c>
       <c r="F49">
         <f>trip_building!H50</f>
         <v>15</v>
@@ -4647,12 +4612,12 @@
         <v>t11 + delta * 2</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9">
       <c r="A50">
         <f>trip_building!C51</f>
         <v>49</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="2">
         <f>trip_building!D51</f>
         <v>44197.387499999997</v>
       </c>
@@ -4664,10 +4629,6 @@
         <f>trip_building!F51</f>
         <v>ATG8613</v>
       </c>
-      <c r="E50">
-        <f>trip_building!G51</f>
-        <v>0</v>
-      </c>
       <c r="F50">
         <f>trip_building!H51</f>
         <v>15</v>
@@ -4685,12 +4646,12 @@
         <v>t11 + delta * 3</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9">
       <c r="A51">
         <f>trip_building!C52</f>
         <v>50</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="2">
         <f>trip_building!D52</f>
         <v>44197.388194444444</v>
       </c>
@@ -4723,12 +4684,12 @@
         <v>t11 + delta * 4</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9">
       <c r="A52">
         <f>trip_building!C53</f>
         <v>51</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="2">
         <f>trip_building!D53</f>
         <v>44197.388888888883</v>
       </c>
@@ -4740,10 +4701,6 @@
         <f>trip_building!F53</f>
         <v>ATGB6I3</v>
       </c>
-      <c r="E52">
-        <f>trip_building!G53</f>
-        <v>0</v>
-      </c>
       <c r="F52">
         <f>trip_building!H53</f>
         <v>15</v>
@@ -4761,12 +4718,12 @@
         <v>t11 + delta * 5</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9">
       <c r="A53">
         <f>trip_building!C54</f>
         <v>52</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="2">
         <f>trip_building!D54</f>
         <v>44197.38958333333</v>
       </c>

</xml_diff>